<commit_message>
adding model for monthly
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestSBO_Replay_Monthly/Model/SBO_MODEL_EVENTS_Replay_Monthly.xlsx
+++ b/src/test/resources/TestDriver/TestSBO_Replay_Monthly/Model/SBO_MODEL_EVENTS_Replay_Monthly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\fyntrac-data-main\fyntrac-data-main\src\test\resources\TestDriver\TestSBO_Replay_Monthly\Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F39FC3-9340-4563-8244-80BD2CCE1BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C354416B-3A1A-4F8B-9EEC-55131CDCC40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TRANX" sheetId="27" r:id="rId1"/>
@@ -1316,8 +1316,8 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2148,7 +2148,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2206,8 +2206,8 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2322,7 +2322,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4321,7 +4321,7 @@
   <dimension ref="A1:XFD58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4426,7 +4426,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="40">
-        <f>IF(B6&lt;&gt;"",COUNT(REPLAY!A2:A29),IF(TRANX!A2&lt;&gt;"",COUNT(TRANX!B2:B29),0))</f>
+        <f>IF(B6&lt;&gt;"",COUNT(REPLAY!A2:A29)+1,IF(TRANX!A2&lt;&gt;"",COUNT(TRANX!B2:B29),0))</f>
         <v>0</v>
       </c>
       <c r="C7" s="38"/>
@@ -17896,7 +17896,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="27" t="str">
-        <f>IF(A13&gt;$B$7,"",IF(REPLAY!B2=$B$5,EOMONTH($B$5,-1),REPLAY!B2))</f>
+        <f>IF(A13&gt;$B$7,"",IF(A13=$B$7,EOMONTH($B$5,-1),REPLAY!B2))</f>
         <v/>
       </c>
       <c r="C13" s="1" t="str">
@@ -17961,7 +17961,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="27" t="str">
-        <f>IF(A14&gt;$B$7,"",IF(REPLAY!B3=$B$5,EOMONTH($B$5,-1),REPLAY!B3))</f>
+        <f>IF(A14&gt;$B$7,"",IF(A14=$B$7,EOMONTH($B$5,-1),REPLAY!B3))</f>
         <v/>
       </c>
       <c r="C14" s="1" t="str">
@@ -18026,7 +18026,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="27" t="str">
-        <f>IF(A15&gt;$B$7,"",IF(REPLAY!B4=$B$5,EOMONTH($B$5,-1),REPLAY!B4))</f>
+        <f>IF(A15&gt;$B$7,"",IF(A15=$B$7,EOMONTH($B$5,-1),REPLAY!B4))</f>
         <v/>
       </c>
       <c r="C15" s="1" t="str">
@@ -18091,7 +18091,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="27" t="str">
-        <f>IF(A16&gt;$B$7,"",IF(REPLAY!B5=$B$5,EOMONTH($B$5,-1),REPLAY!B5))</f>
+        <f>IF(A16&gt;$B$7,"",IF(A16=$B$7,EOMONTH($B$5,-1),REPLAY!B5))</f>
         <v/>
       </c>
       <c r="C16" s="1" t="str">
@@ -18156,7 +18156,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="27" t="str">
-        <f>IF(A17&gt;$B$7,"",IF(REPLAY!B6=$B$5,EOMONTH($B$5,-1),REPLAY!B6))</f>
+        <f>IF(A17&gt;$B$7,"",IF(A17=$B$7,EOMONTH($B$5,-1),REPLAY!B6))</f>
         <v/>
       </c>
       <c r="C17" s="1" t="str">
@@ -18221,7 +18221,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="27" t="str">
-        <f>IF(A18&gt;$B$7,"",IF(REPLAY!B7=$B$5,EOMONTH($B$5,-1),REPLAY!B7))</f>
+        <f>IF(A18&gt;$B$7,"",IF(A18=$B$7,EOMONTH($B$5,-1),REPLAY!B7))</f>
         <v/>
       </c>
       <c r="C18" s="1" t="str">
@@ -18286,7 +18286,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="27" t="str">
-        <f>IF(A19&gt;$B$7,"",IF(REPLAY!B8=$B$5,EOMONTH($B$5,-1),REPLAY!B8))</f>
+        <f>IF(A19&gt;$B$7,"",IF(A19=$B$7,EOMONTH($B$5,-1),REPLAY!B8))</f>
         <v/>
       </c>
       <c r="C19" s="1" t="str">
@@ -18351,7 +18351,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="27" t="str">
-        <f>IF(A20&gt;$B$7,"",IF(REPLAY!B9=$B$5,EOMONTH($B$5,-1),REPLAY!B9))</f>
+        <f>IF(A20&gt;$B$7,"",IF(A20=$B$7,EOMONTH($B$5,-1),REPLAY!B9))</f>
         <v/>
       </c>
       <c r="C20" s="1" t="str">
@@ -18416,7 +18416,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="27" t="str">
-        <f>IF(A21&gt;$B$7,"",IF(REPLAY!B10=$B$5,EOMONTH($B$5,-1),REPLAY!B10))</f>
+        <f>IF(A21&gt;$B$7,"",IF(A21=$B$7,EOMONTH($B$5,-1),REPLAY!B10))</f>
         <v/>
       </c>
       <c r="C21" s="1" t="str">
@@ -18481,7 +18481,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="27" t="str">
-        <f>IF(A22&gt;$B$7,"",IF(REPLAY!B11=$B$5,EOMONTH($B$5,-1),REPLAY!B11))</f>
+        <f>IF(A22&gt;$B$7,"",IF(A22=$B$7,EOMONTH($B$5,-1),REPLAY!B11))</f>
         <v/>
       </c>
       <c r="C22" s="1" t="str">
@@ -18546,7 +18546,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="27" t="str">
-        <f>IF(A23&gt;$B$7,"",IF(REPLAY!B12=$B$5,EOMONTH($B$5,-1),REPLAY!B12))</f>
+        <f>IF(A23&gt;$B$7,"",IF(A23=$B$7,EOMONTH($B$5,-1),REPLAY!B12))</f>
         <v/>
       </c>
       <c r="C23" s="1" t="str">
@@ -18611,7 +18611,7 @@
         <v>12</v>
       </c>
       <c r="B24" s="27" t="str">
-        <f>IF(A24&gt;$B$7,"",IF(REPLAY!B13=$B$5,EOMONTH($B$5,-1),REPLAY!B13))</f>
+        <f>IF(A24&gt;$B$7,"",IF(A24=$B$7,EOMONTH($B$5,-1),REPLAY!B13))</f>
         <v/>
       </c>
       <c r="C24" s="1" t="str">

</xml_diff>

<commit_message>
Checking in test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestSBO_Replay_Monthly/Model/SBO_MODEL_EVENTS_Replay_Monthly.xlsx
+++ b/src/test/resources/TestDriver/TestSBO_Replay_Monthly/Model/SBO_MODEL_EVENTS_Replay_Monthly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\fyntrac-data-main\fyntrac-data-main\src\test\resources\TestDriver\TestSBO_Replay_Monthly\Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65C0251-1EE7-4807-B670-C0C4EC35278E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22681A31-A59E-4D19-9982-26AD46436BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TRANX" sheetId="27" r:id="rId1"/>
@@ -1047,6 +1047,27 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1073,27 +1094,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1363,7 +1363,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F3"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,8 +1507,8 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,16 +1525,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="135" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="130"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="137"/>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="90" t="s">
@@ -1549,22 +1549,22 @@
       <c r="B5" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="137" t="s">
+      <c r="C5" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="138" t="s">
+      <c r="D5" s="129" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="139" t="s">
+      <c r="F5" s="130" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="140" t="s">
+      <c r="G5" s="131" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="139" t="s">
+      <c r="H5" s="130" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1581,8 +1581,8 @@
       <c r="D6" s="6">
         <v>1</v>
       </c>
-      <c r="E6" s="141"/>
-      <c r="F6" s="141"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
       <c r="G6" s="81">
         <v>100000</v>
       </c>
@@ -1929,16 +1929,16 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="128" t="s">
+      <c r="A31" s="135" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="129"/>
-      <c r="C31" s="129"/>
-      <c r="D31" s="129"/>
-      <c r="E31" s="129"/>
-      <c r="F31" s="129"/>
-      <c r="G31" s="129"/>
-      <c r="H31" s="130"/>
+      <c r="B31" s="136"/>
+      <c r="C31" s="136"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="136"/>
+      <c r="F31" s="136"/>
+      <c r="G31" s="136"/>
+      <c r="H31" s="137"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="105" t="s">
@@ -2340,18 +2340,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="H1" s="132" t="s">
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="H1" s="139" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="132"/>
+      <c r="I1" s="139"/>
       <c r="M1" s="6" t="s">
         <v>22</v>
       </c>
@@ -3063,7 +3063,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3178,7 +3178,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:G24"/>
+      <selection activeCell="A27" sqref="A27:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3194,16 +3194,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="53" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="135" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="130"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="137"/>
     </row>
     <row r="2" spans="1:8" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:8" s="53" customFormat="1" ht="21" x14ac:dyDescent="0.35">
@@ -3213,7 +3213,7 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="142" t="s">
+      <c r="A5" s="133" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="78" t="s">
@@ -3234,7 +3234,7 @@
       <c r="G5" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="139" t="s">
+      <c r="H5" s="130" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3242,7 +3242,7 @@
       <c r="A6" s="79">
         <v>44712</v>
       </c>
-      <c r="B6" s="143">
+      <c r="B6" s="134">
         <v>44592</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -3251,8 +3251,8 @@
       <c r="D6" s="6">
         <v>1</v>
       </c>
-      <c r="E6" s="141"/>
-      <c r="F6" s="141"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
       <c r="G6" s="81">
         <v>100000</v>
       </c>
@@ -3579,16 +3579,16 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="128" t="s">
+      <c r="A30" s="135" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="129"/>
-      <c r="C30" s="129"/>
-      <c r="D30" s="129"/>
-      <c r="E30" s="129"/>
-      <c r="F30" s="129"/>
-      <c r="G30" s="129"/>
-      <c r="H30" s="130"/>
+      <c r="B30" s="136"/>
+      <c r="C30" s="136"/>
+      <c r="D30" s="136"/>
+      <c r="E30" s="136"/>
+      <c r="F30" s="136"/>
+      <c r="G30" s="136"/>
+      <c r="H30" s="137"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="105" t="s">
@@ -3973,18 +3973,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="H1" s="132" t="s">
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="H1" s="139" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="132"/>
+      <c r="I1" s="139"/>
       <c r="M1" s="6" t="s">
         <v>22</v>
       </c>
@@ -5194,8 +5194,8 @@
   </sheetPr>
   <dimension ref="A1:XFD58"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5226,19 +5226,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="141" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="135"/>
-      <c r="K1" s="136"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="143"/>
     </row>
     <row r="2" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -5329,24 +5329,24 @@
       <c r="D9" s="38"/>
     </row>
     <row r="10" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="134" t="s">
+      <c r="A10" s="141" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="135"/>
-      <c r="C10" s="135"/>
-      <c r="D10" s="135"/>
-      <c r="E10" s="135"/>
-      <c r="F10" s="135"/>
-      <c r="G10" s="135"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="135"/>
-      <c r="J10" s="135"/>
-      <c r="K10" s="135"/>
-      <c r="L10" s="135"/>
-      <c r="M10" s="135"/>
-      <c r="N10" s="135"/>
-      <c r="O10" s="135"/>
-      <c r="P10" s="136"/>
+      <c r="B10" s="142"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="142"/>
+      <c r="F10" s="142"/>
+      <c r="G10" s="142"/>
+      <c r="H10" s="142"/>
+      <c r="I10" s="142"/>
+      <c r="J10" s="142"/>
+      <c r="K10" s="142"/>
+      <c r="L10" s="142"/>
+      <c r="M10" s="142"/>
+      <c r="N10" s="142"/>
+      <c r="O10" s="142"/>
+      <c r="P10" s="143"/>
     </row>
     <row r="11" spans="1:1024 1026:2048 2050:3072 3074:4096 4098:5120 5122:6144 6146:7168 7170:8192 8194:9216 9218:10240 10242:11264 11266:12288 12290:13312 13314:14336 14338:15360 15362:16384" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="64" t="s">
@@ -19676,24 +19676,24 @@
       <c r="M30" s="41"/>
     </row>
     <row r="31" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="134" t="s">
+      <c r="A31" s="141" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="135"/>
-      <c r="C31" s="135"/>
-      <c r="D31" s="135"/>
-      <c r="E31" s="135"/>
-      <c r="F31" s="135"/>
-      <c r="G31" s="135"/>
-      <c r="H31" s="135"/>
-      <c r="I31" s="135"/>
-      <c r="J31" s="135"/>
-      <c r="K31" s="135"/>
-      <c r="L31" s="135"/>
-      <c r="M31" s="135"/>
-      <c r="N31" s="135"/>
-      <c r="O31" s="135"/>
-      <c r="P31" s="136"/>
+      <c r="B31" s="142"/>
+      <c r="C31" s="142"/>
+      <c r="D31" s="142"/>
+      <c r="E31" s="142"/>
+      <c r="F31" s="142"/>
+      <c r="G31" s="142"/>
+      <c r="H31" s="142"/>
+      <c r="I31" s="142"/>
+      <c r="J31" s="142"/>
+      <c r="K31" s="142"/>
+      <c r="L31" s="142"/>
+      <c r="M31" s="142"/>
+      <c r="N31" s="142"/>
+      <c r="O31" s="142"/>
+      <c r="P31" s="143"/>
     </row>
     <row r="32" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="64" t="s">
@@ -19784,11 +19784,11 @@
         <v/>
       </c>
       <c r="F33" s="28" t="str">
-        <f>IFERROR(IF(B33="","",VLOOKUP(B5,EOD!$B$2:$G$15,5,FALSE)),"")</f>
+        <f>IFERROR(IF(B33="","",VLOOKUP(B5,EOD!$B$2:$G$15,5,FALSE)+D27),"")</f>
         <v/>
       </c>
       <c r="G33" s="28" t="str">
-        <f>IFERROR(IF(B33="","",VLOOKUP(B5,EOD!$B$2:$G$15,6,FALSE)),"")</f>
+        <f>IFERROR(IF(B33="","",VLOOKUP(B5,EOD!$B$2:$G$15,6,FALSE)+D28),"")</f>
         <v/>
       </c>
       <c r="H33" s="6" t="str">
@@ -20867,14 +20867,14 @@
     </row>
     <row r="47" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="133" t="s">
+      <c r="A48" s="140" t="s">
         <v>56</v>
       </c>
-      <c r="B48" s="133"/>
-      <c r="C48" s="133"/>
-      <c r="D48" s="133"/>
-      <c r="E48" s="133"/>
-      <c r="F48" s="133"/>
+      <c r="B48" s="140"/>
+      <c r="C48" s="140"/>
+      <c r="D48" s="140"/>
+      <c r="E48" s="140"/>
+      <c r="F48" s="140"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="51" t="s">
@@ -21078,19 +21078,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="141" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="135"/>
-      <c r="K1" s="136"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="143"/>
       <c r="L1" s="53"/>
       <c r="M1" s="53"/>
       <c r="N1" s="53"/>
@@ -21349,24 +21349,24 @@
       <c r="Y9" s="53"/>
     </row>
     <row r="10" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="134" t="s">
+      <c r="A10" s="141" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="135"/>
-      <c r="C10" s="135"/>
-      <c r="D10" s="135"/>
-      <c r="E10" s="135"/>
-      <c r="F10" s="135"/>
-      <c r="G10" s="135"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="135"/>
-      <c r="J10" s="135"/>
-      <c r="K10" s="135"/>
-      <c r="L10" s="135"/>
-      <c r="M10" s="135"/>
-      <c r="N10" s="135"/>
-      <c r="O10" s="135"/>
-      <c r="P10" s="136"/>
+      <c r="B10" s="142"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="142"/>
+      <c r="F10" s="142"/>
+      <c r="G10" s="142"/>
+      <c r="H10" s="142"/>
+      <c r="I10" s="142"/>
+      <c r="J10" s="142"/>
+      <c r="K10" s="142"/>
+      <c r="L10" s="142"/>
+      <c r="M10" s="142"/>
+      <c r="N10" s="142"/>
+      <c r="O10" s="142"/>
+      <c r="P10" s="143"/>
       <c r="Q10" s="53"/>
       <c r="R10" s="53"/>
       <c r="S10" s="53"/>
@@ -22240,7 +22240,7 @@
       <c r="X25" s="53"/>
       <c r="Y25" s="53"/>
     </row>
-    <row r="26" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>37</v>
       </c>
@@ -22400,24 +22400,24 @@
       <c r="Y30" s="53"/>
     </row>
     <row r="31" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="134" t="s">
+      <c r="A31" s="141" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="135"/>
-      <c r="C31" s="135"/>
-      <c r="D31" s="135"/>
-      <c r="E31" s="135"/>
-      <c r="F31" s="135"/>
-      <c r="G31" s="135"/>
-      <c r="H31" s="135"/>
-      <c r="I31" s="135"/>
-      <c r="J31" s="135"/>
-      <c r="K31" s="135"/>
-      <c r="L31" s="135"/>
-      <c r="M31" s="135"/>
-      <c r="N31" s="135"/>
-      <c r="O31" s="135"/>
-      <c r="P31" s="136"/>
+      <c r="B31" s="142"/>
+      <c r="C31" s="142"/>
+      <c r="D31" s="142"/>
+      <c r="E31" s="142"/>
+      <c r="F31" s="142"/>
+      <c r="G31" s="142"/>
+      <c r="H31" s="142"/>
+      <c r="I31" s="142"/>
+      <c r="J31" s="142"/>
+      <c r="K31" s="142"/>
+      <c r="L31" s="142"/>
+      <c r="M31" s="142"/>
+      <c r="N31" s="142"/>
+      <c r="O31" s="142"/>
+      <c r="P31" s="143"/>
       <c r="Q31" s="53"/>
       <c r="R31" s="53"/>
       <c r="S31" s="53"/>
@@ -23435,14 +23435,14 @@
       <c r="Y47" s="53"/>
     </row>
     <row r="48" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="133" t="s">
+      <c r="A48" s="140" t="s">
         <v>56</v>
       </c>
-      <c r="B48" s="133"/>
-      <c r="C48" s="133"/>
-      <c r="D48" s="133"/>
-      <c r="E48" s="133"/>
-      <c r="F48" s="133"/>
+      <c r="B48" s="140"/>
+      <c r="C48" s="140"/>
+      <c r="D48" s="140"/>
+      <c r="E48" s="140"/>
+      <c r="F48" s="140"/>
       <c r="G48" s="53"/>
       <c r="H48" s="53"/>
       <c r="I48" s="53"/>
@@ -24229,7 +24229,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24429,18 +24429,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="H1" s="132" t="s">
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="H1" s="139" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="132"/>
+      <c r="I1" s="139"/>
       <c r="M1" s="6" t="s">
         <v>22</v>
       </c>

</xml_diff>